<commit_message>
commit de aurelien depuis le pc de thomas (j'avais oublié un détail)
</commit_message>
<xml_diff>
--- a/03enriched_clients_with_charts.xlsx
+++ b/03enriched_clients_with_charts.xlsx
@@ -211,7 +211,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="000000"/>
+              <a:srgbClr val="FF00FF"/>
             </a:solidFill>
           </c:spPr>
           <c:cat>
@@ -365,7 +365,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="000000"/>
+              <a:srgbClr val="0000FF"/>
             </a:solidFill>
           </c:spPr>
           <c:cat>
@@ -519,7 +519,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="FF0000"/>
+              <a:srgbClr val="008000"/>
             </a:solidFill>
           </c:spPr>
           <c:cat>
@@ -673,7 +673,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="008000"/>
+              <a:srgbClr val="FF00FF"/>
             </a:solidFill>
           </c:spPr>
           <c:cat>
@@ -827,7 +827,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="000000"/>
+              <a:srgbClr val="0000FF"/>
             </a:solidFill>
           </c:spPr>
           <c:cat>
@@ -981,7 +981,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="000000"/>
+              <a:srgbClr val="FF0000"/>
             </a:solidFill>
           </c:spPr>
           <c:cat>
@@ -1129,7 +1129,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="008000"/>
+              <a:srgbClr val="FF00FF"/>
             </a:solidFill>
           </c:spPr>
           <c:cat>

</xml_diff>